<commit_message>
feat: login admin double match update
</commit_message>
<xml_diff>
--- a/league_of_ktp.xlsx
+++ b/league_of_ktp.xlsx
@@ -477,13 +477,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>815</v>
+        <v>799</v>
       </c>
       <c r="C2" t="n">
         <v>15</v>
       </c>
       <c r="D2" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -502,10 +502,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1092</v>
+        <v>1107</v>
       </c>
       <c r="C3" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" t="n">
         <v>5</v>
@@ -527,10 +527,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1000</v>
+        <v>1015</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -577,13 +577,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1253</v>
+        <v>1237</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>

</xml_diff>